<commit_message>
added excel sheet for marksheet which is completed
</commit_message>
<xml_diff>
--- a/Debugging Marksheet.xlsx
+++ b/Debugging Marksheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caine\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caine\OneDrive\Desktop\Luftetar_Debugging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83E7C3EB-69AF-4879-A6AD-43C496408413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9754A22D-CFA6-4658-A334-3C99D508680E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0CADD638-67FD-41D1-B5CA-DDC5A7F4EAED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Sr No</t>
   </si>
@@ -66,7 +66,34 @@
     <t>Code_6</t>
   </si>
   <si>
-    <t>Code_7</t>
+    <t>John Sijo</t>
+  </si>
+  <si>
+    <t>Hanushree M</t>
+  </si>
+  <si>
+    <t>Sidharth KS</t>
+  </si>
+  <si>
+    <t>Dhamodharan S P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arshin Joseph Giril </t>
+  </si>
+  <si>
+    <t>Aswin ES</t>
+  </si>
+  <si>
+    <t>Aahil Muhammed</t>
+  </si>
+  <si>
+    <t>Alwin Joshy</t>
+  </si>
+  <si>
+    <t>Naveenkumar T</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -418,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D792D09-EF62-48F7-B316-5DA39F14CF0D}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +457,7 @@
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,60 +489,336 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>40</v>
+      </c>
+      <c r="K2">
+        <v>80</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <f>(D3+E3+F3+G3+H3+I3+J3)</f>
+        <v>74</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <f>(D4+E4+F4+G4+H4+I4+J4)</f>
+        <v>46</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <f>(D5+E5+F5+G5+H5+I5+J5)</f>
+        <v>32</v>
+      </c>
+      <c r="L5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <f>(D6+E6+F6+G6+H6+I6+J6)</f>
+        <v>30</v>
+      </c>
+      <c r="L6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>12</v>
+      </c>
+      <c r="K7">
+        <f>(D7+E7+F7+G7+H7+I7+J7)</f>
+        <v>22</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>20</v>
+      </c>
+      <c r="K8">
+        <f>(D8+E8+F8+G8+H8+I8+J8)</f>
+        <v>20</v>
+      </c>
+      <c r="L8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <f>(D9+E9+F9+G9+H9+I9+J9)</f>
+        <v>12</v>
+      </c>
+      <c r="L9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <f>(D10+E10+F10+G10+H10+I10+J10)</f>
+        <v>12</v>
+      </c>
+      <c r="L10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L10">
+    <sortCondition descending="1" ref="K2:K10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>